<commit_message>
updated mac version to 0.0.0.0.11
</commit_message>
<xml_diff>
--- a/examples/shared.xlsx
+++ b/examples/shared.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5861E-9C0F-6E42-8FD6-90C203A249F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F1009B-1AFF-AC41-99ED-AC056B619086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acls" sheetId="51" r:id="rId1"/>
-    <sheet name="resourcegroups" sheetId="50" r:id="rId2"/>
-    <sheet name="sshkeys" sheetId="36" r:id="rId3"/>
+    <sheet name="resourcegroups" sheetId="50" r:id="rId1"/>
+    <sheet name="sshkeys" sheetId="36" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>*name</t>
   </si>
@@ -42,54 +41,6 @@
   </si>
   <si>
     <t>tags</t>
-  </si>
-  <si>
-    <t>*action</t>
-  </si>
-  <si>
-    <t>*source</t>
-  </si>
-  <si>
-    <t>*destination</t>
-  </si>
-  <si>
-    <t>*direction</t>
-  </si>
-  <si>
-    <t>protocol</t>
-  </si>
-  <si>
-    <t>acl_name</t>
-  </si>
-  <si>
-    <t>iacl1rule100</t>
-  </si>
-  <si>
-    <t>allow</t>
-  </si>
-  <si>
-    <t>0.0.0.0/0</t>
-  </si>
-  <si>
-    <t>inbound</t>
-  </si>
-  <si>
-    <t>tcp:80:80</t>
-  </si>
-  <si>
-    <t>acl1</t>
-  </si>
-  <si>
-    <t>iacl1rule200</t>
-  </si>
-  <si>
-    <t>udp:805:807</t>
-  </si>
-  <si>
-    <t>eacl1rule100</t>
-  </si>
-  <si>
-    <t>outbound</t>
   </si>
 </sst>
 </file>
@@ -119,7 +70,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -127,37 +78,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="8">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -193,43 +130,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -245,31 +145,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:F4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="9"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{379E4E99-C663-0344-AEEB-AA29A196CF21}" name="Table2" displayName="Table2" ref="H1:H2" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="H1:H2" xr:uid="{1E645224-6427-3946-AE0C-8455A88C5D34}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{836016F3-6F84-C442-85F0-7F3A9C84749F}" name="acl_name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40439FC5-EA51-2A47-B328-F7BF6C6013A4}" name="Table32" displayName="Table32" ref="A1:B2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
@@ -280,7 +155,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D18409AA-A6BC-C848-A5DF-F5A05474C1AC}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
@@ -553,112 +428,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB3C17B-7688-8D45-9DEE-F9650DD6901F}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="7" max="7" width="1.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FBFF83-9D9E-6145-AD07-7984EB9C9B1F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -670,10 +439,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -689,7 +458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D3E930-7386-4478-9099-4EC8B39AF425}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -701,10 +470,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>